<commit_message>
small bug fixed, add a new assertion to it
</commit_message>
<xml_diff>
--- a/cook/test/status_report.xlsx
+++ b/cook/test/status_report.xlsx
@@ -1091,8 +1091,8 @@
       <c r="K13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>51</v>
+      <c r="L13" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>50</v>
@@ -1173,8 +1173,8 @@
       <c r="K15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>51</v>
+      <c r="L15" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>50</v>
@@ -1214,8 +1214,8 @@
       <c r="K16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>51</v>
+      <c r="L16" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>50</v>
@@ -1255,8 +1255,8 @@
       <c r="K17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>51</v>
+      <c r="L17" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>50</v>
@@ -1296,8 +1296,8 @@
       <c r="K18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>51</v>
+      <c r="L18" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>50</v>
@@ -1337,8 +1337,8 @@
       <c r="K19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>51</v>
+      <c r="L19" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>50</v>
@@ -1378,8 +1378,8 @@
       <c r="K20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>51</v>
+      <c r="L20" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>50</v>
@@ -1419,8 +1419,8 @@
       <c r="K21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>51</v>
+      <c r="L21" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>50</v>
@@ -1460,8 +1460,8 @@
       <c r="K22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>51</v>
+      <c r="L22" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>50</v>
@@ -1501,8 +1501,8 @@
       <c r="K23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>51</v>
+      <c r="L23" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>50</v>

</xml_diff>